<commit_message>
Actualización automática 2025-05-13 16:40:01
</commit_message>
<xml_diff>
--- a/data/ventas.xlsx
+++ b/data/ventas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\mi_proyecto_python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\mi_proyecto_python\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A57B8E-4BC6-48E9-BFDC-D1E59284A970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E61FF3-4CF1-4993-A28B-C4A5C9649E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4725" yWindow="1980" windowWidth="13905" windowHeight="11940" xr2:uid="{B1BB73B8-1A6F-4728-85F9-F302D2169FD0}"/>
+    <workbookView xWindow="1980" yWindow="3165" windowWidth="22140" windowHeight="13005" xr2:uid="{B1BB73B8-1A6F-4728-85F9-F302D2169FD0}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,72 +25,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
-  <si>
-    <t>Fecha</t>
-  </si>
-  <si>
-    <t>Producto</t>
-  </si>
-  <si>
-    <t>Categoría</t>
-  </si>
-  <si>
-    <t>Región</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Cliente</t>
   </si>
   <si>
-    <t>Unidades</t>
+    <t>Ventas</t>
   </si>
   <si>
-    <t>Precio Unitario</t>
+    <t>Alice</t>
   </si>
   <si>
-    <t>Laptop</t>
+    <t>Bob</t>
   </si>
   <si>
-    <t>Tecnología</t>
-  </si>
-  <si>
-    <t>Bogotá</t>
-  </si>
-  <si>
-    <t>Cliente A</t>
-  </si>
-  <si>
-    <t>3,000,000</t>
-  </si>
-  <si>
-    <t>6,000,000</t>
-  </si>
-  <si>
-    <t>Impresora</t>
-  </si>
-  <si>
-    <t>Medellín</t>
-  </si>
-  <si>
-    <t>Cliente B</t>
-  </si>
-  <si>
-    <t>Escritorio</t>
-  </si>
-  <si>
-    <t>Muebles</t>
-  </si>
-  <si>
-    <t>Cali</t>
-  </si>
-  <si>
-    <t>Cliente C</t>
-  </si>
-  <si>
-    <t>2,000,000</t>
-  </si>
-  <si>
-    <t>ventas</t>
+    <t>Carlos</t>
   </si>
 </sst>
 </file>
@@ -134,7 +83,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -143,6 +92,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -462,114 +414,66 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>45658</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="3">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="B2" s="4">
+        <v>150</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>45658</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="3">
-        <v>1</v>
-      </c>
-      <c r="G3" s="3">
-        <v>800</v>
-      </c>
-      <c r="H3" s="3">
-        <v>800</v>
-      </c>
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="4">
+        <v>200</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>45659</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="3">
-        <v>5</v>
-      </c>
-      <c r="G4" s="3">
-        <v>400</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="4">
+        <v>300</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>